<commit_message>
download excel with sales completed
</commit_message>
<xml_diff>
--- a/Backend/media/planillas_excel/ventas.xlsx
+++ b/Backend/media/planillas_excel/ventas.xlsx
@@ -1,3 +1,146 @@
+
+<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
+  <bookViews>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Datos" sheetId="1" state="visible" r:id="rId1"/>
+  </sheets>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+</workbook>
+</file>
+
+<file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
+    </font>
+  </fonts>
+  <fills count="3">
+    <fill>
+      <patternFill/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00f1f1f1"/>
+        <bgColor rgb="00f1f1f1"/>
+      </patternFill>
+    </fill>
+  </fills>
+  <borders count="1">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+  </borders>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+  </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+  </cellStyles>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
+</styleSheet>
+</file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
@@ -280,4 +423,227 @@
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
+</file>
+
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="21" customWidth="1" min="1" max="1"/>
+    <col width="10" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="9" customWidth="1" min="4" max="4"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Fecha</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Monto</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Metodo de pago</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Usuario</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>2025-12-16 03:08:08</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>2000.0</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>Tarjeta de credito</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>2025-12-16 03:15:12</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>2000.0</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>Tarjeta de debito</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>2025-12-16 03:15:54</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>2000.0</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>Tarjeta de credito</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>2025-12-16 03:29:24</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>196000.0</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>Tarjeta de debito</t>
+        </is>
+      </c>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>2025-12-16 03:32:00</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>200000.0</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>Transferencia</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t>2025-12-16 04:04:19</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>18000.0</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>Tarjeta de debito</t>
+        </is>
+      </c>
+      <c r="D7" s="3" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>2025-12-17 12:12:26</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>9990.0</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>Tarjeta de debito</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="inlineStr">
+        <is>
+          <t>2025-12-17 22:55:30</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>1800.0</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>Tarjeta de credito</t>
+        </is>
+      </c>
+      <c r="D9" s="3" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
change icons to new logo
</commit_message>
<xml_diff>
--- a/Backend/media/planillas_excel/ventas.xlsx
+++ b/Backend/media/planillas_excel/ventas.xlsx
@@ -55,15 +55,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -431,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,8 +437,8 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="21" customWidth="1" min="1" max="1"/>
-    <col width="10" customWidth="1" min="2" max="2"/>
-    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="7" customWidth="1" min="2" max="2"/>
+    <col width="19" customWidth="1" min="3" max="3"/>
     <col width="9" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
@@ -470,174 +467,20 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>2025-12-16 03:08:08</t>
+          <t>2026-02-03 22:05:46</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>2000.0</t>
+          <t>123.0</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>Tarjeta de credito</t>
+          <t>Tarjeta de debito</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
-        <is>
-          <t>admin</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="inlineStr">
-        <is>
-          <t>2025-12-16 03:15:12</t>
-        </is>
-      </c>
-      <c r="B3" s="3" t="inlineStr">
-        <is>
-          <t>2000.0</t>
-        </is>
-      </c>
-      <c r="C3" s="3" t="inlineStr">
-        <is>
-          <t>Tarjeta de debito</t>
-        </is>
-      </c>
-      <c r="D3" s="3" t="inlineStr">
-        <is>
-          <t>admin</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>2025-12-16 03:15:54</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>2000.0</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>Tarjeta de credito</t>
-        </is>
-      </c>
-      <c r="D4" s="2" t="inlineStr">
-        <is>
-          <t>admin</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="inlineStr">
-        <is>
-          <t>2025-12-16 03:29:24</t>
-        </is>
-      </c>
-      <c r="B5" s="3" t="inlineStr">
-        <is>
-          <t>196000.0</t>
-        </is>
-      </c>
-      <c r="C5" s="3" t="inlineStr">
-        <is>
-          <t>Tarjeta de debito</t>
-        </is>
-      </c>
-      <c r="D5" s="3" t="inlineStr">
-        <is>
-          <t>admin</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>2025-12-16 03:32:00</t>
-        </is>
-      </c>
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>200000.0</t>
-        </is>
-      </c>
-      <c r="C6" s="2" t="inlineStr">
-        <is>
-          <t>Transferencia</t>
-        </is>
-      </c>
-      <c r="D6" s="2" t="inlineStr">
-        <is>
-          <t>admin</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="inlineStr">
-        <is>
-          <t>2025-12-16 04:04:19</t>
-        </is>
-      </c>
-      <c r="B7" s="3" t="inlineStr">
-        <is>
-          <t>18000.0</t>
-        </is>
-      </c>
-      <c r="C7" s="3" t="inlineStr">
-        <is>
-          <t>Tarjeta de debito</t>
-        </is>
-      </c>
-      <c r="D7" s="3" t="inlineStr">
-        <is>
-          <t>admin</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="inlineStr">
-        <is>
-          <t>2025-12-17 12:12:26</t>
-        </is>
-      </c>
-      <c r="B8" s="2" t="inlineStr">
-        <is>
-          <t>9990.0</t>
-        </is>
-      </c>
-      <c r="C8" s="2" t="inlineStr">
-        <is>
-          <t>Tarjeta de debito</t>
-        </is>
-      </c>
-      <c r="D8" s="2" t="inlineStr">
-        <is>
-          <t>admin</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="3" t="inlineStr">
-        <is>
-          <t>2025-12-17 22:55:30</t>
-        </is>
-      </c>
-      <c r="B9" s="3" t="inlineStr">
-        <is>
-          <t>1800.0</t>
-        </is>
-      </c>
-      <c r="C9" s="3" t="inlineStr">
-        <is>
-          <t>Tarjeta de credito</t>
-        </is>
-      </c>
-      <c r="D9" s="3" t="inlineStr">
         <is>
           <t>admin</t>
         </is>

</xml_diff>